<commit_message>
REVISIÓN FINAL DE LOS DOCUMENTOS PARA ENTREGA
</commit_message>
<xml_diff>
--- a/DocumentationSprint4/IT/TCO.xlsx
+++ b/DocumentationSprint4/IT/TCO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fjbel\Desktop\universidad\3º\PSG2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fjbc1\git\PSG2-2021-G5-51\DocumentationSprint4\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AA8E69-4B44-4270-B7E0-42DE74DFACE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D8902E-F297-4936-80D4-39224FEA2356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCO ROI - BLANK" sheetId="3" r:id="rId1"/>
@@ -27,8 +27,17 @@
     <definedName name="Type" localSheetId="0">'[1]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -48,9 +57,6 @@
     <t>Year 3</t>
   </si>
   <si>
-    <t>Peripherals</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -135,9 +141,6 @@
     <t>Development Tools Licensing PY</t>
   </si>
   <si>
-    <t>Unicamente cuesta 10'50 € cada desarrollado mensualmente</t>
-  </si>
-  <si>
     <t>3 miembros del equipo cobrando mensualmente 2.500 €</t>
   </si>
   <si>
@@ -159,10 +162,16 @@
     <t>Gestión software anual</t>
   </si>
   <si>
-    <t>Precio de los perifericos: 5 equipos, un teclado, 5 ratones, 3 auriculares y 2 pantallas</t>
-  </si>
-  <si>
-    <t>Migración de la información e almacenamiento</t>
+    <t>Únicamente cuesta 10'50 € cada herramienta mensualmente</t>
+  </si>
+  <si>
+    <t>Hardware and Peripherals</t>
+  </si>
+  <si>
+    <t>Migración de la información e almacenamiento en logs</t>
+  </si>
+  <si>
+    <t>Precio de: 5 equipos, un teclado, 5 ratones, 3 auriculares y 2 pantallas. Incluye costes de renovación en caso de avería, obsolescencia, etc.</t>
   </si>
 </sst>
 </file>
@@ -170,9 +179,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -372,13 +381,13 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -395,22 +404,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -419,13 +428,13 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -437,7 +446,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -752,32 +761,32 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.75" style="1" customWidth="1"/>
-    <col min="3" max="6" width="18.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="65.375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.69921875" style="1" customWidth="1"/>
+    <col min="3" max="6" width="18.69921875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="65.3984375" style="14" customWidth="1"/>
     <col min="8" max="8" width="31" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3.25" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.75" style="1"/>
+    <col min="9" max="9" width="3.19921875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>0</v>
@@ -789,15 +798,15 @@
         <v>2</v>
       </c>
       <c r="F2" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -805,9 +814,9 @@
       <c r="F3" s="17"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="18">
         <v>90000</v>
@@ -823,12 +832,12 @@
         <v>270000</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="18">
         <v>43000</v>
@@ -844,12 +853,12 @@
         <v>129000</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="20">
         <f>SUM(C3:C5)</f>
@@ -869,9 +878,9 @@
       </c>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -879,9 +888,9 @@
       <c r="F7" s="17"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="18">
         <v>630</v>
@@ -897,54 +906,54 @@
         <v>1890</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="19">
         <f t="shared" ref="F9:F11" si="1">SUM(C9:E9)</f>
         <v>0</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="21">
         <v>70000</v>
@@ -960,12 +969,12 @@
         <v>210000</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="20">
         <f>SUM(C8:C11)</f>
@@ -985,9 +994,9 @@
       </c>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -995,9 +1004,9 @@
       <c r="F13" s="17"/>
       <c r="G13" s="23"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="18">
         <v>12000</v>
@@ -1013,12 +1022,12 @@
         <v>36000</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="18">
         <v>24000</v>
@@ -1034,12 +1043,12 @@
         <v>72000</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="18">
         <v>110000</v>
@@ -1055,12 +1064,12 @@
         <v>330000</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="20">
         <f>SUM(C13:C16)</f>
@@ -1080,21 +1089,21 @@
       </c>
       <c r="G17" s="23"/>
     </row>
-    <row r="18" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="23"/>
     </row>
-    <row r="19" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C19" s="18">
         <v>5890</v>
@@ -1110,12 +1119,12 @@
         <v>5890</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="20">
         <f>SUM(C19)</f>
@@ -1135,9 +1144,9 @@
       </c>
       <c r="G20" s="23"/>
     </row>
-    <row r="21" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -1145,9 +1154,9 @@
       <c r="F21" s="17"/>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="31">
         <v>500</v>
@@ -1163,12 +1172,12 @@
         <v>1500</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="5" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="20">
         <f>SUM(C22)</f>
@@ -1188,7 +1197,7 @@
       </c>
       <c r="G23" s="24"/>
     </row>
-    <row r="24" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" s="5" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1196,9 +1205,9 @@
       <c r="F24" s="8"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:7" s="5" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" s="5" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="22">
         <f>SUM(C23,C20,C17,C12,C6,)</f>
@@ -1218,17 +1227,17 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="2:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="10"/>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1236,7 +1245,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" s="4" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1244,16 +1253,16 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1261,7 +1270,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="2:7" s="5" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" s="5" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1269,141 +1278,141 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="16"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="16"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="16"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="16"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="16"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="16"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="16"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="16"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="16"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="16"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="16"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="16"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="2:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="2:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="15"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="7:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="7:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="7:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="7:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="7:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="7:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="7:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="7:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="7:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="7:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="7:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="7:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="7:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="7:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="7:7" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="7:7" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="7:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="7:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="7:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="7:7" ht="15" x14ac:dyDescent="0.25">
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="7:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="7:7" ht="15" x14ac:dyDescent="0.25">
       <c r="G75" s="1"/>
     </row>
   </sheetData>

</xml_diff>